<commit_message>
regional statistics pipeline finished
</commit_message>
<xml_diff>
--- a/dictionaries/decoding_dict.xlsx
+++ b/dictionaries/decoding_dict.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4ba23d5b7de37717/MADS/IST737/project/dictionaries/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="180" documentId="11_F25DC773A252ABDACC104888C19C6AFE5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BC278601-299B-4EF4-AB6D-7F5A67069A9F}"/>
+  <xr:revisionPtr revIDLastSave="196" documentId="11_F25DC773A252ABDACC104888C19C6AFE5BDE58F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70F2DE76-8DFA-406C-8DA1-8F55608BA22A}"/>
   <bookViews>
-    <workbookView xWindow="3495" yWindow="3495" windowWidth="21600" windowHeight="11385" tabRatio="902" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7200" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="902" firstSheet="1" activeTab="16" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="age" sheetId="1" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <sheet name="frequenc" sheetId="14" r:id="rId14"/>
     <sheet name="quantile" sheetId="15" r:id="rId15"/>
     <sheet name="unit" sheetId="16" r:id="rId16"/>
+    <sheet name="victim" sheetId="17" r:id="rId17"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="314">
   <si>
     <t>From 16 to 19 years</t>
   </si>
@@ -963,6 +964,36 @@
   </si>
   <si>
     <t>GE3</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Inhabitants per ...</t>
+  </si>
+  <si>
+    <t>Per hundred thousand inhabitants</t>
+  </si>
+  <si>
+    <t>NR</t>
+  </si>
+  <si>
+    <t>HAB_P</t>
+  </si>
+  <si>
+    <t>P_HTHAB</t>
+  </si>
+  <si>
+    <t>KIL</t>
+  </si>
+  <si>
+    <t>INJ</t>
+  </si>
+  <si>
+    <t>Killed</t>
+  </si>
+  <si>
+    <t>Injured</t>
   </si>
 </sst>
 </file>
@@ -1928,10 +1959,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2475D2-9F43-4B7D-8DB1-CFDF846B5F99}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1959,6 +1990,72 @@
       <c r="B3" t="s">
         <v>233</v>
       </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="B4" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="B5" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B6" t="s">
+        <v>306</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D8E51C5-7966-48C6-8505-9205E569550C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B2" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1969,7 +2066,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D47EF05D-786E-45AD-A8F3-796212A99DC9}">
   <dimension ref="A1:B46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>

</xml_diff>